<commit_message>
working on adding specialty table
</commit_message>
<xml_diff>
--- a/VinList.xlsx
+++ b/VinList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horva\Documents\vinDecodingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{114B1C1A-DBB5-4BB7-9957-FB54D8504F93}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6C8DBFEA-4D0C-4269-940F-43DCC4EA2C15}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="8376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>2NPNHD6X93M808079</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>VIN</t>
+  </si>
+  <si>
+    <t>4V4NC9EJ2EN168028</t>
   </si>
 </sst>
 </file>
@@ -950,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B26" sqref="B26:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1170,6 +1173,14 @@
         <v>100116</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1">
+        <v>100116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added second specialty database into backend
</commit_message>
<xml_diff>
--- a/VinList.xlsx
+++ b/VinList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horva\Documents\vinDecodingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6C8DBFEA-4D0C-4269-940F-43DCC4EA2C15}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E5E10DD1-7C1E-4A49-AB48-03CAE61F6EEA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="8376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>2NPNHD6X93M808079</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>4V4NC9EJ2EN168028</t>
+  </si>
+  <si>
+    <t>4V4MC9DG8DN542142</t>
   </si>
 </sst>
 </file>
@@ -953,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B27"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1181,6 +1184,14 @@
         <v>100116</v>
       </c>
     </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1">
+        <v>100116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
commit before adding customer vin/ cindy vin BOM decoding
</commit_message>
<xml_diff>
--- a/VinList.xlsx
+++ b/VinList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horva\Documents\vinDecodingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E5E10DD1-7C1E-4A49-AB48-03CAE61F6EEA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E76EC890-78BE-4EDE-8A6F-CAFCB3E860A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="8376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -958,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
requires variable clean up
</commit_message>
<xml_diff>
--- a/VinList.xlsx
+++ b/VinList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horva\Documents\vinDecodingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E76EC890-78BE-4EDE-8A6F-CAFCB3E860A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0039475F-E612-4627-B854-069D1EC26374}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="8376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -959,7 +959,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1020,39 +1020,39 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>100116</v>
+      <c r="B7">
+        <v>100038</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
-        <v>100116</v>
+      <c r="B8">
+        <v>100080</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>100116</v>
+      <c r="B9">
+        <v>100081</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
-        <v>100116</v>
+      <c r="B10">
+        <v>100112</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>100116</v>
       </c>
     </row>
@@ -1060,16 +1060,16 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
-        <v>100116</v>
+      <c r="B12">
+        <v>100118</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
-        <v>100116</v>
+      <c r="B13">
+        <v>100120</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">

</xml_diff>